<commit_message>
working revision of gaussian vary_system experiment
</commit_message>
<xml_diff>
--- a/cms_system_200.xlsx
+++ b/cms_system_200.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D4B645-9213-2747-BE83-790FB1C00817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF07DF-E672-AF45-A35F-C317A9815CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="4000" windowWidth="25560" windowHeight="21340" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="51020" yWindow="12080" windowWidth="21600" windowHeight="21340" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Category</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Reduction Ratio</t>
+  </si>
+  <si>
+    <t>Classifier</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>L1T</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -223,9 +235,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,7 +275,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -369,7 +381,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,15 +1090,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50D47B-EF5E-D84A-888D-0FD7C5F25128}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1100,22 +1112,25 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1128,23 +1143,26 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>43</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1157,23 +1175,26 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>43</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
       <c r="I3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1186,23 +1207,26 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>43</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1215,23 +1239,26 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -1244,23 +1271,26 @@
       <c r="D6" s="2">
         <v>53.3</v>
       </c>
-      <c r="E6" s="2">
-        <v>3</v>
+      <c r="E6" t="s">
+        <v>42</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1273,23 +1303,26 @@
       <c r="D7" s="2">
         <v>100</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>16</v>
       </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1300,19 +1333,22 @@
       <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
+      <c r="E8" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
         <v>2.5000000000000001E-11</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
       <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating plots and figures
</commit_message>
<xml_diff>
--- a/cms_system_200.xlsx
+++ b/cms_system_200.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF07DF-E672-AF45-A35F-C317A9815CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8B6C6-A62C-F945-ABD1-DD346703184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51020" yWindow="12080" windowWidth="21600" windowHeight="21340" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="17860" yWindow="29560" windowWidth="21600" windowHeight="17380" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -533,12 +533,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -1092,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50D47B-EF5E-D84A-888D-0FD7C5F25128}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding HLT data and upates
</commit_message>
<xml_diff>
--- a/cms_system_200.xlsx
+++ b/cms_system_200.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD8B6C6-A62C-F945-ABD1-DD346703184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056B708D-227F-E642-91E1-7945042B9853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17860" yWindow="29560" windowWidth="21600" windowHeight="17380" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="51800" yWindow="7580" windowWidth="21600" windowHeight="17380" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50D47B-EF5E-D84A-888D-0FD7C5F25128}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="A1:J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
new results table with calibrated HLT
</commit_message>
<xml_diff>
--- a/cms_system_200.xlsx
+++ b/cms_system_200.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056B708D-227F-E642-91E1-7945042B9853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05DB4E3-742E-C841-97C3-5CCFE075E28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51800" yWindow="7580" windowWidth="21600" windowHeight="17380" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="-24620" yWindow="5160" windowWidth="21600" windowHeight="17380" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -163,13 +163,13 @@
     <t>Classifier</t>
   </si>
   <si>
-    <t>Gaussian</t>
-  </si>
-  <si>
     <t>L1T</t>
   </si>
   <si>
     <t>Dummy</t>
+  </si>
+  <si>
+    <t>HLT</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1241,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>53.3</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>

</xml_diff>